<commit_message>
Random forest model tuning
</commit_message>
<xml_diff>
--- a/data/caver_models/CastP_submission_log_manual.xlsx
+++ b/data/caver_models/CastP_submission_log_manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robi0916/Documents/University_of_Minnesota/Wackett_Lab/github/synbio-data-analysis/data/caver_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9272400C-4C99-774B-9D7A-636DA7295D81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6326F6C7-681E-3748-9109-71514108268D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13820"/>
+    <workbookView xWindow="-53420" yWindow="640" windowWidth="30660" windowHeight="25220"/>
   </bookViews>
   <sheets>
     <sheet name="CastP_submission_log" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="170">
   <si>
     <t>ABL00697_1_Pelobacter_propionicus_DSM_2379.pdb</t>
   </si>
@@ -274,9 +274,6 @@
     <t>Radius (Å)</t>
   </si>
   <si>
-    <t>j_5e0fa8de03c37</t>
-  </si>
-  <si>
     <t>j_5e0fa90c2c423</t>
   </si>
   <si>
@@ -397,9 +394,6 @@
     <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fb3999e2d0</t>
   </si>
   <si>
-    <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fb3c382551</t>
-  </si>
-  <si>
     <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fb3d5f0771</t>
   </si>
   <si>
@@ -448,9 +442,6 @@
     <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fb52f969ac</t>
   </si>
   <si>
-    <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fb5428a008</t>
-  </si>
-  <si>
     <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fb590db0e3</t>
   </si>
   <si>
@@ -484,17 +475,80 @@
     <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fb649bef87</t>
   </si>
   <si>
-    <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fb6573318b</t>
-  </si>
-  <si>
-    <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fb6a82dd47</t>
+    <t>http://sts.bioe.uic.edu/castp/index.html?j_5e10318c10cb7</t>
+  </si>
+  <si>
+    <t>http://sts.bioe.uic.edu/castp/index.html?j_5e1031b487421</t>
+  </si>
+  <si>
+    <t>http://sts.bioe.uic.edu/castp/index.html?j_5e0fa8de03c37</t>
+  </si>
+  <si>
+    <t>Huge bulbous protrusion from the P channel</t>
+  </si>
+  <si>
+    <t>To keep</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Another bulbous P-channel protrusion</t>
+  </si>
+  <si>
+    <t>Appears to not have a B channel</t>
+  </si>
+  <si>
+    <t>Only one channel detected</t>
+  </si>
+  <si>
+    <t>P channel protrusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weird shape, protrusion </t>
+  </si>
+  <si>
+    <t>http://sts.bioe.uic.edu/castp/index.html?j_5e10359b2cbf9</t>
+  </si>
+  <si>
+    <t>No observable B channel</t>
+  </si>
+  <si>
+    <t>Did not detect P channel</t>
+  </si>
+  <si>
+    <t>Large A channel protrusion</t>
+  </si>
+  <si>
+    <t>P channel not detected</t>
+  </si>
+  <si>
+    <t>A channel protrusion, P channel not detected</t>
+  </si>
+  <si>
+    <t>B channel not detected</t>
+  </si>
+  <si>
+    <t>Channel in wrong place</t>
+  </si>
+  <si>
+    <t>A channel protrusion</t>
+  </si>
+  <si>
+    <t>Weird B channel/P channel merge</t>
+  </si>
+  <si>
+    <t>http://sts.bioe.uic.edu/castp/index.html?j_5e103a9f4e71b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -636,6 +690,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -986,12 +1046,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1348,20 +1409,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="70.83203125" customWidth="1"/>
     <col min="2" max="2" width="51.83203125" customWidth="1"/>
-    <col min="4" max="5" width="13" customWidth="1"/>
+    <col min="4" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -1378,10 +1439,13 @@
         <v>79</v>
       </c>
       <c r="F1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1398,15 +1462,18 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="F2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
+      <c r="B3" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="C3" s="2">
         <v>561.40200000000004</v>
@@ -1417,619 +1484,1498 @@
       <c r="E3" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="C4" s="5">
+        <v>776.39499999999998</v>
+      </c>
+      <c r="D4" s="5">
+        <v>780.87599999999998</v>
       </c>
       <c r="E4" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="C5" s="5">
+        <v>253.49700000000001</v>
+      </c>
+      <c r="D5" s="5">
+        <v>115.92100000000001</v>
       </c>
       <c r="E5" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="C6" s="5">
+        <v>555.57299999999998</v>
+      </c>
+      <c r="D6" s="5">
+        <v>415.82400000000001</v>
       </c>
       <c r="E6" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="C7" s="5">
+        <v>286.87799999999999</v>
+      </c>
+      <c r="D7" s="5">
+        <v>184.35400000000001</v>
       </c>
       <c r="E7" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="C8" s="5">
+        <v>232.20400000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <v>120.45099999999999</v>
       </c>
       <c r="E8" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="C9" s="5">
+        <v>451.37400000000002</v>
+      </c>
+      <c r="D9" s="5">
+        <v>211.19200000000001</v>
       </c>
       <c r="E9" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C10" s="5">
+        <v>425.96899999999999</v>
+      </c>
+      <c r="D10" s="5">
+        <v>275.464</v>
       </c>
       <c r="E10" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="C11" s="5">
+        <v>407.09100000000001</v>
+      </c>
+      <c r="D11" s="5">
+        <v>182.328</v>
       </c>
       <c r="E11" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="C12" s="5">
+        <v>171.90299999999999</v>
+      </c>
+      <c r="D12" s="5">
+        <v>51.412999999999997</v>
       </c>
       <c r="E12" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C13" s="5">
+        <v>551.10900000000004</v>
+      </c>
+      <c r="D13" s="5">
+        <v>344.66</v>
       </c>
       <c r="E13" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="C14" s="5">
+        <v>500.26</v>
+      </c>
+      <c r="D14" s="5">
+        <v>304.78500000000003</v>
       </c>
       <c r="E14" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="C15" s="5">
+        <v>306.78300000000002</v>
+      </c>
+      <c r="D15" s="5">
+        <v>291.78500000000003</v>
       </c>
       <c r="E15" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="C16" s="5">
+        <v>260.495</v>
+      </c>
+      <c r="D16" s="5">
+        <v>95.259</v>
       </c>
       <c r="E16" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="C17" s="5">
+        <v>347.57</v>
+      </c>
+      <c r="D17" s="5">
+        <v>226.02</v>
       </c>
       <c r="E17" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>151</v>
+        <v>159</v>
+      </c>
+      <c r="C18">
+        <v>496.00900000000001</v>
+      </c>
+      <c r="D18">
+        <v>230.708</v>
       </c>
       <c r="E18" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="C19" s="5">
+        <v>537.31700000000001</v>
+      </c>
+      <c r="D19" s="5">
+        <v>277.05700000000002</v>
       </c>
       <c r="E19" s="4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="C20" s="5">
+        <v>257.899</v>
+      </c>
+      <c r="D20" s="5">
+        <v>135.018</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="C21" s="5">
+        <v>462.84500000000003</v>
+      </c>
+      <c r="D21" s="5">
+        <v>212.321</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="C22" s="5">
+        <v>437.78</v>
+      </c>
+      <c r="D22" s="5">
+        <v>204.203</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="C23" s="5">
+        <v>437.78</v>
+      </c>
+      <c r="D23" s="5">
+        <v>204.203</v>
+      </c>
+      <c r="E23" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="C24" s="5">
+        <v>502.37599999999998</v>
+      </c>
+      <c r="D24" s="5">
+        <v>253.86</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="C25" s="5">
+        <v>425.517</v>
+      </c>
+      <c r="D25" s="5">
+        <v>200.13900000000001</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="5">
+        <v>556.245</v>
+      </c>
+      <c r="D26" s="5">
+        <v>300.33699999999999</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="C27" s="5">
+        <v>477.488</v>
+      </c>
+      <c r="D27" s="5">
+        <v>248.185</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="C28" s="5">
+        <v>459.75299999999999</v>
+      </c>
+      <c r="D28" s="5">
+        <v>217.78100000000001</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="C29" s="5">
+        <v>547.16499999999996</v>
+      </c>
+      <c r="D29" s="5">
+        <v>329.22199999999998</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="C30" s="5">
+        <v>360.80700000000002</v>
+      </c>
+      <c r="D30" s="5">
+        <v>182.56100000000001</v>
+      </c>
+      <c r="E30" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="C31" s="5">
+        <v>299.41399999999999</v>
+      </c>
+      <c r="D31" s="5">
+        <v>169.15799999999999</v>
+      </c>
+      <c r="E31" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="C32" s="5">
+        <v>502.178</v>
+      </c>
+      <c r="D32" s="5">
+        <v>234.93600000000001</v>
+      </c>
+      <c r="E32" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="C33" s="5">
+        <v>519.96400000000006</v>
+      </c>
+      <c r="D33" s="5">
+        <v>304.73</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="C34" s="5">
+        <v>395.529</v>
+      </c>
+      <c r="D34" s="5">
+        <v>188.83799999999999</v>
+      </c>
+      <c r="E34" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="C35" s="5">
+        <v>457.23700000000002</v>
+      </c>
+      <c r="D35" s="5">
+        <v>200.39500000000001</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="C36" s="5">
+        <v>397.24400000000003</v>
+      </c>
+      <c r="D36" s="5">
+        <v>201.71600000000001</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="C37" s="5">
+        <v>60.523000000000003</v>
+      </c>
+      <c r="D37" s="5">
+        <v>165.733</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F37" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="C38" s="5">
+        <v>453.13200000000001</v>
+      </c>
+      <c r="D38" s="5">
+        <v>208.72800000000001</v>
+      </c>
+      <c r="E38" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="C39" s="5">
+        <v>472.88</v>
+      </c>
+      <c r="D39" s="5">
+        <v>249.92500000000001</v>
+      </c>
+      <c r="E39" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="C40" s="5">
+        <v>468.084</v>
+      </c>
+      <c r="D40" s="5">
+        <v>213.631</v>
+      </c>
+      <c r="E40" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="C41" s="5">
+        <v>491.43599999999998</v>
+      </c>
+      <c r="D41" s="5">
+        <v>228.92500000000001</v>
+      </c>
+      <c r="E41" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="C42" s="5">
+        <v>429.28300000000002</v>
+      </c>
+      <c r="D42" s="5">
+        <v>274.56200000000001</v>
+      </c>
+      <c r="E42" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="C43" s="5">
+        <v>657.00800000000004</v>
+      </c>
+      <c r="D43" s="5">
+        <v>478.9</v>
+      </c>
+      <c r="E43" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="C44" s="5">
+        <v>491.37799999999999</v>
+      </c>
+      <c r="D44" s="5">
+        <v>228.90299999999999</v>
+      </c>
+      <c r="E44" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="C45" s="5">
+        <v>259.93599999999998</v>
+      </c>
+      <c r="D45" s="5">
+        <v>102.52800000000001</v>
+      </c>
+      <c r="E45" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G45" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="C46" s="5">
+        <v>311.13099999999997</v>
+      </c>
+      <c r="D46" s="5">
+        <v>148.76599999999999</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="C47" s="5">
+        <v>511.01600000000002</v>
+      </c>
+      <c r="D47" s="5">
+        <v>282.154</v>
+      </c>
+      <c r="E47" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="C48" s="5">
+        <v>336.63099999999997</v>
+      </c>
+      <c r="D48" s="5">
+        <v>158.99299999999999</v>
+      </c>
+      <c r="E48" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="C49" s="5">
+        <v>479.476</v>
+      </c>
+      <c r="D49" s="5">
+        <v>235.89</v>
+      </c>
+      <c r="E49" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="C50" s="5">
+        <v>390.94200000000001</v>
+      </c>
+      <c r="D50" s="5">
+        <v>186.08699999999999</v>
+      </c>
+      <c r="E50" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="C51" s="5">
+        <v>484.94400000000002</v>
+      </c>
+      <c r="D51" s="5">
+        <v>230.494</v>
+      </c>
+      <c r="E51" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="C52" s="5">
+        <v>491.43599999999998</v>
+      </c>
+      <c r="D52" s="5">
+        <v>228.92500000000001</v>
+      </c>
+      <c r="E52" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+      <c r="C53" s="5">
+        <v>395.81400000000002</v>
+      </c>
+      <c r="D53" s="5">
+        <v>159.62899999999999</v>
+      </c>
+      <c r="E53" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G53" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="C54" s="5">
+        <v>563.47900000000004</v>
+      </c>
+      <c r="D54" s="5">
+        <v>243.565</v>
+      </c>
+      <c r="E54" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="C55" s="5">
+        <v>369.94099999999997</v>
+      </c>
+      <c r="D55" s="5">
+        <v>201.38499999999999</v>
+      </c>
+      <c r="E55" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="C56" s="5">
+        <v>410.39299999999997</v>
+      </c>
+      <c r="D56" s="5">
+        <v>164.69300000000001</v>
+      </c>
+      <c r="E56" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="C57" s="5">
+        <v>449.46199999999999</v>
+      </c>
+      <c r="D57" s="5">
+        <v>223.166</v>
+      </c>
+      <c r="E57" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G57" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="C58" s="5">
+        <v>454.88499999999999</v>
+      </c>
+      <c r="D58" s="5">
+        <v>234.42699999999999</v>
+      </c>
+      <c r="E58" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="C59" s="5">
+        <v>497.25200000000001</v>
+      </c>
+      <c r="D59" s="5">
+        <v>215.18199999999999</v>
+      </c>
+      <c r="E59" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="C60" s="5">
+        <v>547.05899999999997</v>
+      </c>
+      <c r="D60" s="5">
+        <v>220.21299999999999</v>
+      </c>
+      <c r="E60" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G60" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="C61" s="5">
+        <v>613.40099999999995</v>
+      </c>
+      <c r="D61" s="5">
+        <v>457.71</v>
+      </c>
+      <c r="E61" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+      <c r="C62" s="5">
+        <v>547.33600000000001</v>
+      </c>
+      <c r="D62" s="5">
+        <v>267.74400000000003</v>
+      </c>
+      <c r="E62" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="C63" s="5">
+        <v>434.70100000000002</v>
+      </c>
+      <c r="D63" s="5">
+        <v>205.86799999999999</v>
+      </c>
+      <c r="E63" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="C64" s="5">
+        <v>576.09500000000003</v>
+      </c>
+      <c r="D64" s="5">
+        <v>257.839</v>
+      </c>
+      <c r="E64" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G64" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="C65" s="5">
+        <v>426.83</v>
+      </c>
+      <c r="D65" s="5">
+        <v>203.99299999999999</v>
+      </c>
+      <c r="E65" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="C66" s="5">
+        <v>511.06</v>
+      </c>
+      <c r="D66" s="5">
+        <v>244.381</v>
+      </c>
+      <c r="E66" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="C67" s="5">
+        <v>579.18700000000001</v>
+      </c>
+      <c r="D67" s="5">
+        <v>303.61900000000003</v>
+      </c>
+      <c r="E67" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="C68" s="5">
+        <v>451.37400000000002</v>
+      </c>
+      <c r="D68" s="5">
+        <v>211.19200000000001</v>
+      </c>
+      <c r="E68" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="C69" s="5">
+        <v>504.68799999999999</v>
+      </c>
+      <c r="D69" s="5">
+        <v>230.749</v>
+      </c>
+      <c r="E69" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+      <c r="C70" s="5">
+        <v>500.24799999999999</v>
+      </c>
+      <c r="D70" s="5">
+        <v>234.27600000000001</v>
+      </c>
+      <c r="E70" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="C71" s="5">
+        <v>448.435</v>
+      </c>
+      <c r="D71" s="5">
+        <v>263.34899999999999</v>
+      </c>
+      <c r="E71" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G71" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="C72" s="5">
+        <v>629.94399999999996</v>
+      </c>
+      <c r="D72" s="5">
+        <v>344.88299999999998</v>
+      </c>
+      <c r="E72" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G72" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="C73" s="5">
+        <v>497.41699999999997</v>
+      </c>
+      <c r="D73" s="5">
+        <v>230.98</v>
+      </c>
+      <c r="E73" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2070,37 +3016,39 @@
     <hyperlink ref="B41" r:id="rId31"/>
     <hyperlink ref="B42" r:id="rId32"/>
     <hyperlink ref="B43" r:id="rId33"/>
-    <hyperlink ref="B44" r:id="rId34"/>
-    <hyperlink ref="B45" r:id="rId35"/>
-    <hyperlink ref="B46" r:id="rId36"/>
-    <hyperlink ref="B47" r:id="rId37"/>
-    <hyperlink ref="B48" r:id="rId38"/>
-    <hyperlink ref="B49" r:id="rId39"/>
-    <hyperlink ref="B50" r:id="rId40"/>
-    <hyperlink ref="B51" r:id="rId41"/>
-    <hyperlink ref="B52" r:id="rId42"/>
-    <hyperlink ref="B53" r:id="rId43"/>
-    <hyperlink ref="B54" r:id="rId44"/>
-    <hyperlink ref="B55" r:id="rId45"/>
-    <hyperlink ref="B56" r:id="rId46"/>
-    <hyperlink ref="B57" r:id="rId47"/>
-    <hyperlink ref="B58" r:id="rId48"/>
-    <hyperlink ref="B59" r:id="rId49"/>
-    <hyperlink ref="B60" r:id="rId50"/>
-    <hyperlink ref="B61" r:id="rId51"/>
-    <hyperlink ref="B62" r:id="rId52"/>
-    <hyperlink ref="B63" r:id="rId53"/>
-    <hyperlink ref="B64" r:id="rId54"/>
-    <hyperlink ref="B65" r:id="rId55"/>
-    <hyperlink ref="B66" r:id="rId56"/>
-    <hyperlink ref="B67" r:id="rId57"/>
-    <hyperlink ref="B68" r:id="rId58"/>
-    <hyperlink ref="B69" r:id="rId59"/>
-    <hyperlink ref="B70" r:id="rId60"/>
-    <hyperlink ref="B71" r:id="rId61"/>
-    <hyperlink ref="B72" r:id="rId62"/>
-    <hyperlink ref="B73" r:id="rId63"/>
+    <hyperlink ref="B45" r:id="rId34"/>
+    <hyperlink ref="B46" r:id="rId35"/>
+    <hyperlink ref="B47" r:id="rId36"/>
+    <hyperlink ref="B48" r:id="rId37"/>
+    <hyperlink ref="B49" r:id="rId38"/>
+    <hyperlink ref="B50" r:id="rId39"/>
+    <hyperlink ref="B51" r:id="rId40"/>
+    <hyperlink ref="B52" r:id="rId41"/>
+    <hyperlink ref="B53" r:id="rId42"/>
+    <hyperlink ref="B54" r:id="rId43"/>
+    <hyperlink ref="B55" r:id="rId44"/>
+    <hyperlink ref="B56" r:id="rId45"/>
+    <hyperlink ref="B57" r:id="rId46"/>
+    <hyperlink ref="B58" r:id="rId47"/>
+    <hyperlink ref="B59" r:id="rId48"/>
+    <hyperlink ref="B60" r:id="rId49"/>
+    <hyperlink ref="B62" r:id="rId50"/>
+    <hyperlink ref="B63" r:id="rId51"/>
+    <hyperlink ref="B64" r:id="rId52"/>
+    <hyperlink ref="B65" r:id="rId53"/>
+    <hyperlink ref="B66" r:id="rId54"/>
+    <hyperlink ref="B67" r:id="rId55"/>
+    <hyperlink ref="B68" r:id="rId56"/>
+    <hyperlink ref="B69" r:id="rId57"/>
+    <hyperlink ref="B70" r:id="rId58"/>
+    <hyperlink ref="B71" r:id="rId59"/>
+    <hyperlink ref="B72" r:id="rId60"/>
+    <hyperlink ref="B44" r:id="rId61"/>
+    <hyperlink ref="B73" r:id="rId62"/>
+    <hyperlink ref="B3" r:id="rId63"/>
     <hyperlink ref="B18" r:id="rId64"/>
+    <hyperlink ref="B26" r:id="rId65"/>
+    <hyperlink ref="B61" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>